<commit_message>
[progress]update progress of 《大话数据结构》
</commit_message>
<xml_diff>
--- a/书目进度.xlsx
+++ b/书目进度.xlsx
@@ -41,12 +41,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -161,7 +162,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -195,6 +196,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -551,7 +555,7 @@
   <dimension ref="A1:DC46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25"/>
@@ -564,7 +568,8 @@
     <col min="6" max="6" width="12.875" style="3" customWidth="1"/>
     <col min="7" max="7" width="9.25" style="4" customWidth="1"/>
     <col min="8" max="8" width="3.5" style="4" customWidth="1"/>
-    <col min="9" max="107" width="3.66666666666667" style="4" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="4" customWidth="1"/>
+    <col min="10" max="107" width="3.66666666666667" style="4" customWidth="1"/>
     <col min="108" max="16381" width="10.8333333333333" style="5"/>
   </cols>
   <sheetData>
@@ -904,7 +909,7 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -916,22 +921,25 @@
       </c>
       <c r="D3" s="8">
         <f>E3/C3</f>
-        <v>0.0620985010706638</v>
+        <v>0.107066381156317</v>
       </c>
       <c r="E3" s="7">
-        <f>MAX(G3:DC3)</f>
-        <v>29</v>
+        <f>SUM(G3:DC3)</f>
+        <v>50</v>
       </c>
       <c r="F3" s="9">
-        <f>(C3-E3)/25</f>
-        <v>17.52</v>
+        <f>(C3-E3)/AVERAGE(I3:DC3)</f>
+        <v>19.8571428571429</v>
       </c>
       <c r="G3" s="10">
         <f>B3</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="4:8">
+      <c r="I3" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9">
       <c r="D4" s="8"/>
       <c r="E4" s="7"/>
       <c r="F4" s="9"/>
@@ -939,6 +947,9 @@
         <v>42056</v>
       </c>
       <c r="H4" s="10"/>
+      <c r="I4" s="13">
+        <v>42056</v>
+      </c>
     </row>
     <row r="5" spans="4:6">
       <c r="D5" s="12"/>

</xml_diff>

<commit_message>
* [progress]update progress of 《大话数据结构》 读完链表
</commit_message>
<xml_diff>
--- a/书目进度.xlsx
+++ b/书目进度.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19820" windowHeight="8360" tabRatio="500"/>
+    <workbookView windowWidth="19800" windowHeight="7940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -42,10 +42,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="177" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
@@ -64,16 +64,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color indexed="20"/>
+      <color indexed="8"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
-      <color indexed="8"/>
+      <color indexed="20"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -152,10 +152,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -163,42 +163,42 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -209,8 +209,8 @@
     <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
     <cellStyle name="百分比" xfId="4" builtinId="5"/>
     <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="普通" xfId="6"/>
-    <cellStyle name="访问过的超链接" xfId="7"/>
+    <cellStyle name="访问过的超链接" xfId="6"/>
+    <cellStyle name="普通" xfId="7"/>
     <cellStyle name="超链接" xfId="8" builtinId="8"/>
   </cellStyles>
 </styleSheet>
@@ -555,7 +555,7 @@
   <dimension ref="A1:DC46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25"/>
@@ -568,8 +568,10 @@
     <col min="6" max="6" width="12.875" style="3" customWidth="1"/>
     <col min="7" max="7" width="9.25" style="4" customWidth="1"/>
     <col min="8" max="8" width="3.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="7.5" style="4" customWidth="1"/>
-    <col min="10" max="107" width="3.66666666666667" style="4" customWidth="1"/>
+    <col min="9" max="10" width="7.5" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="7.5" style="4" customWidth="1"/>
+    <col min="13" max="107" width="3.66666666666667" style="4" customWidth="1"/>
     <col min="108" max="16381" width="10.8333333333333" style="5"/>
   </cols>
   <sheetData>
@@ -909,7 +911,7 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -921,15 +923,15 @@
       </c>
       <c r="D3" s="8">
         <f>E3/C3</f>
-        <v>0.107066381156317</v>
+        <v>0.246252676659529</v>
       </c>
       <c r="E3" s="7">
         <f>SUM(G3:DC3)</f>
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="F3" s="9">
         <f>(C3-E3)/AVERAGE(I3:DC3)</f>
-        <v>19.8571428571429</v>
+        <v>16.3720930232558</v>
       </c>
       <c r="G3" s="10">
         <f>B3</f>
@@ -938,8 +940,17 @@
       <c r="I3" s="4">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="4:9">
+      <c r="J3" s="4">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4">
+        <v>13</v>
+      </c>
+      <c r="L3" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="4:107">
       <c r="D4" s="8"/>
       <c r="E4" s="7"/>
       <c r="F4" s="9"/>
@@ -950,6 +961,110 @@
       <c r="I4" s="13">
         <v>42056</v>
       </c>
+      <c r="J4" s="13">
+        <v>42057</v>
+      </c>
+      <c r="K4" s="13">
+        <v>42058</v>
+      </c>
+      <c r="L4" s="13">
+        <v>42059</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="13"/>
+      <c r="BA4" s="13"/>
+      <c r="BB4" s="13"/>
+      <c r="BC4" s="13"/>
+      <c r="BD4" s="13"/>
+      <c r="BE4" s="13"/>
+      <c r="BF4" s="13"/>
+      <c r="BG4" s="13"/>
+      <c r="BH4" s="13"/>
+      <c r="BI4" s="13"/>
+      <c r="BJ4" s="13"/>
+      <c r="BK4" s="13"/>
+      <c r="BL4" s="13"/>
+      <c r="BM4" s="13"/>
+      <c r="BN4" s="13"/>
+      <c r="BO4" s="13"/>
+      <c r="BP4" s="13"/>
+      <c r="BQ4" s="13"/>
+      <c r="BR4" s="13"/>
+      <c r="BS4" s="13"/>
+      <c r="BT4" s="13"/>
+      <c r="BU4" s="13"/>
+      <c r="BV4" s="13"/>
+      <c r="BW4" s="13"/>
+      <c r="BX4" s="13"/>
+      <c r="BY4" s="13"/>
+      <c r="BZ4" s="13"/>
+      <c r="CA4" s="13"/>
+      <c r="CB4" s="13"/>
+      <c r="CC4" s="13"/>
+      <c r="CD4" s="13"/>
+      <c r="CE4" s="13"/>
+      <c r="CF4" s="13"/>
+      <c r="CG4" s="13"/>
+      <c r="CH4" s="13"/>
+      <c r="CI4" s="13"/>
+      <c r="CJ4" s="13"/>
+      <c r="CK4" s="13"/>
+      <c r="CL4" s="13"/>
+      <c r="CM4" s="13"/>
+      <c r="CN4" s="13"/>
+      <c r="CO4" s="13"/>
+      <c r="CP4" s="13"/>
+      <c r="CQ4" s="13"/>
+      <c r="CR4" s="13"/>
+      <c r="CS4" s="13"/>
+      <c r="CT4" s="13"/>
+      <c r="CU4" s="13"/>
+      <c r="CV4" s="13"/>
+      <c r="CW4" s="13"/>
+      <c r="CX4" s="13"/>
+      <c r="CY4" s="13"/>
+      <c r="CZ4" s="13"/>
+      <c r="DA4" s="13"/>
+      <c r="DB4" s="13"/>
+      <c r="DC4" s="13"/>
     </row>
     <row r="5" spans="4:6">
       <c r="D5" s="12"/>
@@ -977,13 +1092,10 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="4:75">
+    <row r="9" spans="4:6">
       <c r="D9" s="12"/>
       <c r="E9" s="7"/>
       <c r="F9" s="9"/>
-      <c r="BW9" s="4">
-        <v>538</v>
-      </c>
     </row>
     <row r="10" spans="4:6">
       <c r="D10" s="8"/>

</xml_diff>

<commit_message>
[progress]update progress of 《大话数据结构》 达成
</commit_message>
<xml_diff>
--- a/书目进度.xlsx
+++ b/书目进度.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="7940" tabRatio="500"/>
+    <workbookView windowWidth="19820" windowHeight="8360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -42,8 +42,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0"/>
@@ -64,16 +64,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="12"/>
-      <color indexed="8"/>
+      <color indexed="20"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color indexed="20"/>
+      <color indexed="8"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -152,10 +152,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -163,42 +163,42 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -209,8 +209,8 @@
     <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
     <cellStyle name="百分比" xfId="4" builtinId="5"/>
     <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="访问过的超链接" xfId="6"/>
-    <cellStyle name="普通" xfId="7"/>
+    <cellStyle name="普通" xfId="6"/>
+    <cellStyle name="访问过的超链接" xfId="7"/>
     <cellStyle name="超链接" xfId="8" builtinId="8"/>
   </cellStyles>
 </styleSheet>
@@ -555,7 +555,7 @@
   <dimension ref="A1:DC46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25"/>
@@ -570,8 +570,9 @@
     <col min="8" max="8" width="3.5" style="4" customWidth="1"/>
     <col min="9" max="10" width="7.5" style="4" customWidth="1"/>
     <col min="11" max="11" width="8.375" style="4" customWidth="1"/>
-    <col min="12" max="14" width="7.5" style="4" customWidth="1"/>
-    <col min="15" max="107" width="3.66666666666667" style="4" customWidth="1"/>
+    <col min="12" max="18" width="7.5" style="4" customWidth="1"/>
+    <col min="19" max="22" width="6.625" style="4" customWidth="1"/>
+    <col min="23" max="107" width="3.66666666666667" style="4" customWidth="1"/>
     <col min="108" max="16381" width="10.8333333333333" style="5"/>
   </cols>
   <sheetData>
@@ -911,7 +912,7 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -923,15 +924,15 @@
       </c>
       <c r="D3" s="8">
         <f>E3/C3</f>
-        <v>0.376873661670236</v>
+        <v>1</v>
       </c>
       <c r="E3" s="7">
         <f>SUM(G3:DC3)</f>
-        <v>176</v>
+        <v>467</v>
       </c>
       <c r="F3" s="9">
         <f>(C3-E3)/AVERAGE(I3:DC3)</f>
-        <v>11.8775510204082</v>
+        <v>0</v>
       </c>
       <c r="G3" s="10">
         <f>B3</f>
@@ -954,6 +955,30 @@
       </c>
       <c r="N3" s="4">
         <v>26</v>
+      </c>
+      <c r="O3" s="4">
+        <v>20</v>
+      </c>
+      <c r="P3" s="4">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>22</v>
+      </c>
+      <c r="R3" s="4">
+        <v>28</v>
+      </c>
+      <c r="S3" s="4">
+        <v>32</v>
+      </c>
+      <c r="T3" s="4">
+        <v>67</v>
+      </c>
+      <c r="U3" s="4">
+        <v>33</v>
+      </c>
+      <c r="V3" s="4">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="4:107">
@@ -982,14 +1007,30 @@
       <c r="N4" s="13">
         <v>42060</v>
       </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
+      <c r="O4" s="13">
+        <v>42061</v>
+      </c>
+      <c r="P4" s="13">
+        <v>42062</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>42062</v>
+      </c>
+      <c r="R4" s="13">
+        <v>42063</v>
+      </c>
+      <c r="S4" s="13">
+        <v>42063</v>
+      </c>
+      <c r="T4" s="13">
+        <v>42063</v>
+      </c>
+      <c r="U4" s="13">
+        <v>42065</v>
+      </c>
+      <c r="V4" s="13">
+        <v>42066</v>
+      </c>
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>

</xml_diff>

<commit_message>
[progress]update progress of 《大话设计模式》
</commit_message>
<xml_diff>
--- a/书目进度.xlsx
+++ b/书目进度.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
   <si>
     <t>书目</t>
   </si>
@@ -36,17 +36,20 @@
   <si>
     <t>大话数据结构</t>
   </si>
+  <si>
+    <t>大话设计模式</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
   <fonts count="10">
@@ -555,7 +558,7 @@
   <dimension ref="A1:DC46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25"/>
@@ -1117,17 +1120,66 @@
       <c r="DB4" s="13"/>
       <c r="DC4" s="13"/>
     </row>
-    <row r="5" spans="4:6">
-      <c r="D5" s="12"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="4:8">
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1">
+        <v>386</v>
+      </c>
+      <c r="D5" s="8">
+        <f>E5/C5</f>
+        <v>0.160621761658031</v>
+      </c>
+      <c r="E5" s="7">
+        <f>SUM(G5:DC5)</f>
+        <v>62</v>
+      </c>
+      <c r="F5" s="9">
+        <f>(C5-E5)/AVERAGE(I5:DC5)</f>
+        <v>15.0697674418605</v>
+      </c>
+      <c r="G5" s="10">
+        <f>B5</f>
+        <v>19</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5" s="4">
+        <v>15</v>
+      </c>
+      <c r="J5" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="4:22">
       <c r="D6" s="8"/>
       <c r="E6" s="7"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="11">
+        <v>42069</v>
+      </c>
       <c r="H6" s="10"/>
+      <c r="I6" s="13">
+        <v>42070</v>
+      </c>
+      <c r="J6" s="13">
+        <v>42071</v>
+      </c>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
     </row>
     <row r="7" spans="4:8">
       <c r="D7" s="8"/>
@@ -1333,8 +1385,9 @@
   <sortState caseSensitive="0" columnSort="0" ref="A3:DF45">
     <sortCondition descending="0" ref="F3:F45"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>